<commit_message>
add description for empiries
</commit_message>
<xml_diff>
--- a/The Rurik Empire/docs/empires.xlsx
+++ b/The Rurik Empire/docs/empires.xlsx
@@ -13,17 +13,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1718785800" val="976" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1718785800" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1718785800" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1718785800"/>
+      <pm:revision xmlns:pm="smNativeData" day="1718787160" val="976" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1718787160" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1718787160" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1718787160"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="196">
   <si>
     <t>id</t>
   </si>
@@ -272,12 +272,41 @@
     <t>Папская область</t>
   </si>
   <si>
+    <t>Теократическое государство, существовавшее в центральной Италии и возглавлявшееся папами ― патриархами Римской Католической церкви.</t>
+  </si>
+  <si>
+    <t>0.055</t>
+  </si>
+  <si>
+    <t>Рим</t>
+  </si>
+  <si>
     <t>Астурия</t>
   </si>
   <si>
+    <t>Автономное сообщество и провинция на севере Испании. Королевство было известно как Астурия до 924 года, затем оно стало называться Королевство Леон.
+Королевство Леон, в свою очередь, в 1230 году было объединено в Королевство Кастилия и Леон.</t>
+  </si>
+  <si>
+    <t>0.070</t>
+  </si>
+  <si>
+    <t>Овьедо</t>
+  </si>
+  <si>
     <t>Кордовский Эмират</t>
   </si>
   <si>
+    <t>Исламское государство на территории Иберийского полуострова, в средневековой Испании (756—929).
+Государство основано потомком Омейядов Абд ар-Рахманом I, который в 756 году принял титул эмира.</t>
+  </si>
+  <si>
+    <t>0.880</t>
+  </si>
+  <si>
+    <t>Кордова</t>
+  </si>
+  <si>
     <t>Королевство Италия</t>
   </si>
   <si>
@@ -585,6 +614,9 @@
   </si>
   <si>
     <t>Гольштейн</t>
+  </si>
+  <si>
+    <t>Кордовский Халифат</t>
   </si>
 </sst>
 </file>
@@ -610,7 +642,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1718785800" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1718787160" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -626,7 +658,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1718785800" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1718787160" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -648,7 +680,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1718785800" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1718787160" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -670,7 +702,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1718785800"/>
+          <pm:border xmlns:pm="smNativeData" id="1718787160"/>
         </ext>
       </extLst>
     </border>
@@ -689,7 +721,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1718785800"/>
+          <pm:border xmlns:pm="smNativeData" id="1718787160"/>
         </ext>
       </extLst>
     </border>
@@ -709,7 +741,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1718785800" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1718787160" count="1">
         <pm:charStyle name="Обычный" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -973,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E126"/>
+  <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="B127" sqref="B127"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
@@ -1310,7 +1342,10 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="1:5">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
       <c r="B20" t="s">
         <v>76</v>
       </c>
@@ -1324,541 +1359,894 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="2:2">
+    <row r="21" spans="1:5">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
       <c r="B21" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="22" spans="2:2">
+      <c r="C21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
       <c r="B22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="n">
         <v>81</v>
       </c>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" t="s">
+      <c r="B82" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="n">
         <v>82</v>
       </c>
-    </row>
-    <row r="24" spans="2:2">
-      <c r="B24" t="s">
+      <c r="B83" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="n">
         <v>83</v>
       </c>
-    </row>
-    <row r="25" spans="2:2">
-      <c r="B25" t="s">
+      <c r="B84" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="n">
         <v>84</v>
       </c>
-    </row>
-    <row r="26" spans="2:2">
-      <c r="B26" t="s">
+      <c r="B85" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="n">
         <v>85</v>
       </c>
-    </row>
-    <row r="27" spans="2:2">
-      <c r="B27" t="s">
+      <c r="B86" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="n">
         <v>86</v>
       </c>
-    </row>
-    <row r="28" spans="2:2">
-      <c r="B28" t="s">
+      <c r="B87" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="n">
         <v>87</v>
       </c>
-    </row>
-    <row r="29" spans="2:2">
-      <c r="B29" t="s">
+      <c r="B88" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="n">
         <v>88</v>
       </c>
-    </row>
-    <row r="30" spans="2:2">
-      <c r="B30" t="s">
+      <c r="B89" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="n">
         <v>89</v>
       </c>
-    </row>
-    <row r="31" spans="2:2">
-      <c r="B31" t="s">
+      <c r="B90" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="n">
         <v>90</v>
       </c>
-    </row>
-    <row r="32" spans="2:2">
-      <c r="B32" t="s">
+      <c r="B91" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="n">
         <v>91</v>
       </c>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" t="s">
+      <c r="B92" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="n">
         <v>92</v>
       </c>
-    </row>
-    <row r="34" spans="2:2">
-      <c r="B34" t="s">
+      <c r="B93" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="n">
         <v>93</v>
       </c>
-    </row>
-    <row r="35" spans="2:2">
-      <c r="B35" t="s">
+      <c r="B94" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="n">
         <v>94</v>
       </c>
-    </row>
-    <row r="36" spans="2:2">
-      <c r="B36" t="s">
+      <c r="B95" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="n">
         <v>95</v>
       </c>
-    </row>
-    <row r="37" spans="2:2">
-      <c r="B37" t="s">
+      <c r="B96" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="n">
         <v>96</v>
       </c>
-    </row>
-    <row r="38" spans="2:2">
-      <c r="B38" t="s">
+      <c r="B97" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="n">
         <v>97</v>
       </c>
-    </row>
-    <row r="39" spans="2:2">
-      <c r="B39" t="s">
+      <c r="B98" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="n">
         <v>98</v>
       </c>
-    </row>
-    <row r="40" spans="2:2">
-      <c r="B40" t="s">
+      <c r="B99" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="n">
         <v>99</v>
       </c>
-    </row>
-    <row r="41" spans="2:2">
-      <c r="B41" t="s">
+      <c r="B100" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="n">
         <v>100</v>
       </c>
-    </row>
-    <row r="42" spans="2:2">
-      <c r="B42" t="s">
+      <c r="B101" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="n">
         <v>101</v>
       </c>
-    </row>
-    <row r="43" spans="2:2">
-      <c r="B43" t="s">
+      <c r="B102" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="n">
         <v>102</v>
       </c>
-    </row>
-    <row r="44" spans="2:2">
-      <c r="B44" t="s">
+      <c r="B103" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="n">
         <v>103</v>
       </c>
-    </row>
-    <row r="45" spans="2:2">
-      <c r="B45" t="s">
+      <c r="B104" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="n">
         <v>104</v>
       </c>
-    </row>
-    <row r="46" spans="2:2">
-      <c r="B46" t="s">
+      <c r="B105" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="n">
         <v>105</v>
       </c>
-    </row>
-    <row r="47" spans="2:2">
-      <c r="B47" t="s">
+      <c r="B106" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="n">
         <v>106</v>
       </c>
-    </row>
-    <row r="48" spans="2:2">
-      <c r="B48" t="s">
+      <c r="B107" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="n">
         <v>107</v>
       </c>
-    </row>
-    <row r="49" spans="2:2">
-      <c r="B49" t="s">
+      <c r="B108" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="n">
         <v>108</v>
       </c>
-    </row>
-    <row r="50" spans="2:2">
-      <c r="B50" t="s">
+      <c r="B109" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="n">
         <v>109</v>
       </c>
-    </row>
-    <row r="51" spans="2:2">
-      <c r="B51" t="s">
+      <c r="B110" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="n">
         <v>110</v>
       </c>
-    </row>
-    <row r="52" spans="2:2">
-      <c r="B52" t="s">
+      <c r="B111" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="n">
         <v>111</v>
       </c>
-    </row>
-    <row r="53" spans="2:2">
-      <c r="B53" t="s">
+      <c r="B112" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="n">
         <v>112</v>
       </c>
-    </row>
-    <row r="54" spans="2:2">
-      <c r="B54" t="s">
+      <c r="B113" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="n">
         <v>113</v>
       </c>
-    </row>
-    <row r="55" spans="2:2">
-      <c r="B55" t="s">
+      <c r="B114" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="n">
         <v>114</v>
       </c>
-    </row>
-    <row r="56" spans="2:2">
-      <c r="B56" t="s">
+      <c r="B115" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="n">
         <v>115</v>
       </c>
-    </row>
-    <row r="57" spans="2:2">
-      <c r="B57" t="s">
+      <c r="B116" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="n">
         <v>116</v>
       </c>
-    </row>
-    <row r="58" spans="2:2">
-      <c r="B58" t="s">
+      <c r="B117" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="n">
         <v>117</v>
       </c>
-    </row>
-    <row r="59" spans="2:2">
-      <c r="B59" t="s">
+      <c r="B118" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="n">
         <v>118</v>
       </c>
-    </row>
-    <row r="60" spans="2:2">
-      <c r="B60" t="s">
+      <c r="B119" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="n">
         <v>119</v>
       </c>
-    </row>
-    <row r="61" spans="2:2">
-      <c r="B61" t="s">
+      <c r="B120" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="n">
         <v>120</v>
       </c>
-    </row>
-    <row r="62" spans="2:2">
-      <c r="B62" t="s">
+      <c r="B121" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" t="n">
         <v>121</v>
       </c>
-    </row>
-    <row r="63" spans="2:2">
-      <c r="B63" t="s">
+      <c r="B122" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" t="n">
         <v>122</v>
       </c>
-    </row>
-    <row r="64" spans="2:2">
-      <c r="B64" t="s">
+      <c r="B123" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" t="n">
         <v>123</v>
       </c>
-    </row>
-    <row r="65" spans="2:2">
-      <c r="B65" t="s">
+      <c r="B124" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" t="n">
         <v>124</v>
       </c>
-    </row>
-    <row r="66" spans="2:2">
-      <c r="B66" t="s">
+      <c r="B125" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" t="n">
         <v>125</v>
       </c>
-    </row>
-    <row r="67" spans="2:2">
-      <c r="B67" t="s">
+      <c r="B126" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" t="n">
         <v>126</v>
       </c>
-    </row>
-    <row r="68" spans="2:2">
-      <c r="B68" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="69" spans="2:2">
-      <c r="B69" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="70" spans="2:2">
-      <c r="B70" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="71" spans="2:2">
-      <c r="B71" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="72" spans="2:2">
-      <c r="B72" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="73" spans="2:2">
-      <c r="B73" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="74" spans="2:2">
-      <c r="B74" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="75" spans="2:2">
-      <c r="B75" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="76" spans="2:2">
-      <c r="B76" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="77" spans="2:2">
-      <c r="B77" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="78" spans="2:2">
-      <c r="B78" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="79" spans="2:2">
-      <c r="B79" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="80" spans="2:2">
-      <c r="B80" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2">
-      <c r="B81" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="82" spans="2:2">
-      <c r="B82" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2">
-      <c r="B83" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="84" spans="2:2">
-      <c r="B84" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="85" spans="2:2">
-      <c r="B85" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="86" spans="2:2">
-      <c r="B86" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="87" spans="2:2">
-      <c r="B87" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="88" spans="2:2">
-      <c r="B88" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="89" spans="2:2">
-      <c r="B89" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="90" spans="2:2">
-      <c r="B90" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="91" spans="2:2">
-      <c r="B91" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="92" spans="2:2">
-      <c r="B92" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="93" spans="2:2">
-      <c r="B93" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="94" spans="2:2">
-      <c r="B94" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="95" spans="2:2">
-      <c r="B95" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="96" spans="2:2">
-      <c r="B96" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="97" spans="2:2">
-      <c r="B97" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="98" spans="2:2">
-      <c r="B98" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="99" spans="2:2">
-      <c r="B99" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="100" spans="2:2">
-      <c r="B100" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="101" spans="2:2">
-      <c r="B101" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="102" spans="2:2">
-      <c r="B102" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="103" spans="2:2">
-      <c r="B103" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="104" spans="2:2">
-      <c r="B104" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="105" spans="2:2">
-      <c r="B105" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="106" spans="2:2">
-      <c r="B106" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="107" spans="2:2">
-      <c r="B107" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="108" spans="2:2">
-      <c r="B108" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="109" spans="2:2">
-      <c r="B109" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="110" spans="2:2">
-      <c r="B110" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="111" spans="2:2">
-      <c r="B111" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="112" spans="2:2">
-      <c r="B112" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="113" spans="2:2">
-      <c r="B113" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="114" spans="2:2">
-      <c r="B114" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="115" spans="2:2">
-      <c r="B115" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="116" spans="2:2">
-      <c r="B116" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="117" spans="2:2">
-      <c r="B117" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="118" spans="2:2">
-      <c r="B118" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="119" spans="2:2">
-      <c r="B119" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="120" spans="2:2">
-      <c r="B120" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="121" spans="2:2">
-      <c r="B121" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="122" spans="2:2">
-      <c r="B122" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="123" spans="2:2">
-      <c r="B123" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="124" spans="2:2">
-      <c r="B124" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="125" spans="2:2">
-      <c r="B125" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="126" spans="2:2">
-      <c r="B126" t="s">
-        <v>185</v>
+      <c r="B127" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1718785800" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1718787160" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1867,16 +2255,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1718785800" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1718785800" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1718785800" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1718785800" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1718787160" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1718787160" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1718787160" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1718787160" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1718785800" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1718787160" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>